<commit_message>
Fix matching mistake with Spartina alterniflora x maritima
</commit_message>
<xml_diff>
--- a/data-raw/DFV_app_indicator_common_species.xlsx
+++ b/data-raw/DFV_app_indicator_common_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au650181_uni_au_dk/Documents/generel/github/FloraExam/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{29915B81-D0A1-4B5D-81C3-323B73AC7152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C3BE46A-C31A-4A17-945A-10153F38C3F5}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{29915B81-D0A1-4B5D-81C3-323B73AC7152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB78C4C0-E729-48E1-A497-29DBB0E732ED}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="1395" windowWidth="28800" windowHeight="15285" xr2:uid="{6724E4C6-8DA9-49C4-962A-E3CD14D84949}"/>
+    <workbookView xWindow="2025" yWindow="3060" windowWidth="17670" windowHeight="11040" xr2:uid="{6724E4C6-8DA9-49C4-962A-E3CD14D84949}"/>
   </bookViews>
   <sheets>
     <sheet name="vascular_plants" sheetId="1" r:id="rId1"/>
@@ -11308,14 +11308,14 @@
     <t>spartina_alterniflora_x_maritima.jpg</t>
   </si>
   <si>
-    <t>Spartina alterniflora x maritima</t>
+    <t>Spartina alterniflora × maritima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11394,8 +11394,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11438,6 +11442,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -11457,10 +11466,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -11552,9 +11562,13 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{5F5A07B6-2663-4C30-8CD8-64848AF97147}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -11572,6 +11586,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11873,9 +11891,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B10A51-DA4A-4AE5-9025-27203DF1119C}">
   <dimension ref="A1:BF616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G440" sqref="G440"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A449" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G454" sqref="G454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -39530,7 +39548,7 @@
       <c r="F453" s="1">
         <v>66027</v>
       </c>
-      <c r="G453" s="2" t="s">
+      <c r="G453" s="31" t="s">
         <v>3741</v>
       </c>
       <c r="H453" s="1" t="s">

</xml_diff>